<commit_message>
Minor change to tracking
Credit TDF team for appropriate updates to ADSL dataset
</commit_message>
<xml_diff>
--- a/data/TRACKING_Comments_TDF_Packages.xlsx
+++ b/data/TRACKING_Comments_TDF_Packages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GiacomoGo\Work\GitHub\phuse-scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC611B2-EB43-405C-BA47-9D0A559CB014}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AECBA0B-7688-4BC8-83FA-A19A84EA522C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22395" windowHeight="11265" xr2:uid="{91F4970D-346D-4276-A6FF-88136B289A12}"/>
   </bookViews>
@@ -86,53 +86,6 @@
     <t xml:space="preserve">adsl.xpt </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">rename DCREASCD to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DCSREAS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, and create new </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EOSSTT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "End of Study Status" column</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">advs.xpt </t>
   </si>
   <si>
@@ -445,6 +398,53 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> in column G (open/closed)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TDF team renamed DCREASCD to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DCSREAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and created new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EOSSTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "End of Study Status" column</t>
     </r>
   </si>
 </sst>
@@ -548,7 +548,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="88">
     <dxf>
       <font>
         <strike val="0"/>
@@ -678,6 +678,230 @@
         <strike val="0"/>
         <color theme="1" tint="0.499984740745262"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -724,246 +948,6 @@
         <strike val="0"/>
         <color theme="1" tint="0.499984740745262"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1234,446 +1218,11 @@
         <strike val="0"/>
         <color theme="1" tint="0.499984740745262"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2016,7 +1565,7 @@
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78" style="1" customWidth="1"/>
+    <col min="4" max="4" width="89.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2057,7 +1606,7 @@
         <v>43450</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>8</v>
@@ -2074,7 +1623,7 @@
         <v>43450</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>8</v>
@@ -2091,7 +1640,7 @@
         <v>43450</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>8</v>
@@ -2108,7 +1657,7 @@
         <v>43450</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>8</v>
@@ -2125,7 +1674,7 @@
         <v>43450</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>8</v>
@@ -2142,7 +1691,7 @@
         <v>43450</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>8</v>
@@ -2159,13 +1708,13 @@
         <v>43450</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2176,7 +1725,7 @@
         <v>43450</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>8</v>
@@ -2193,10 +1742,10 @@
         <v>43450</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2210,10 +1759,10 @@
         <v>43450</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,10 +1776,10 @@
         <v>43450</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2244,13 +1793,13 @@
         <v>43450</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -2261,15 +1810,15 @@
         <v>43450</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
@@ -2278,10 +1827,10 @@
         <v>43450</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2351,13 +1900,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="G29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2376,170 +1925,170 @@
     <sortCondition ref="A2:A15"/>
   </sortState>
   <conditionalFormatting sqref="G2:G28">
-    <cfRule type="cellIs" dxfId="155" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="77" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
       <formula>"closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:F28">
-    <cfRule type="expression" dxfId="151" priority="63">
+    <cfRule type="expression" dxfId="85" priority="63">
       <formula>$G15="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="64">
+    <cfRule type="expression" dxfId="84" priority="64">
       <formula>$G15="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:F14">
-    <cfRule type="expression" dxfId="85" priority="37">
+    <cfRule type="expression" dxfId="83" priority="37">
       <formula>$G14="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="38">
+    <cfRule type="expression" dxfId="82" priority="38">
       <formula>$G14="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:F13">
-    <cfRule type="expression" dxfId="83" priority="35">
+    <cfRule type="expression" dxfId="81" priority="35">
       <formula>$G13="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="36">
+    <cfRule type="expression" dxfId="80" priority="36">
       <formula>$G13="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:F12">
-    <cfRule type="expression" dxfId="81" priority="33">
+    <cfRule type="expression" dxfId="79" priority="33">
       <formula>$G12="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="34">
+    <cfRule type="expression" dxfId="78" priority="34">
       <formula>$G12="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:F11">
-    <cfRule type="expression" dxfId="79" priority="31">
+    <cfRule type="expression" dxfId="77" priority="31">
       <formula>$G11="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="32">
+    <cfRule type="expression" dxfId="76" priority="32">
       <formula>$G11="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:F10">
-    <cfRule type="expression" dxfId="77" priority="29">
+    <cfRule type="expression" dxfId="75" priority="29">
       <formula>$G10="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="30">
+    <cfRule type="expression" dxfId="74" priority="30">
       <formula>$G10="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:F9">
-    <cfRule type="expression" dxfId="75" priority="27">
+    <cfRule type="expression" dxfId="73" priority="27">
       <formula>$G9="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="28">
+    <cfRule type="expression" dxfId="72" priority="28">
       <formula>$G9="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 E8:F8">
-    <cfRule type="expression" dxfId="73" priority="25">
+    <cfRule type="expression" dxfId="71" priority="25">
       <formula>$G8="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="26">
+    <cfRule type="expression" dxfId="70" priority="26">
       <formula>$G8="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C7 E7:F7">
-    <cfRule type="expression" dxfId="71" priority="23">
+    <cfRule type="expression" dxfId="69" priority="23">
       <formula>$G7="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="24">
+    <cfRule type="expression" dxfId="68" priority="24">
       <formula>$G7="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:C6 E6:F6">
-    <cfRule type="expression" dxfId="69" priority="21">
+    <cfRule type="expression" dxfId="67" priority="21">
       <formula>$G6="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="22">
+    <cfRule type="expression" dxfId="66" priority="22">
       <formula>$G6="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:F5">
-    <cfRule type="expression" dxfId="67" priority="19">
+    <cfRule type="expression" dxfId="65" priority="19">
       <formula>$G5="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="20">
+    <cfRule type="expression" dxfId="64" priority="20">
       <formula>$G5="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="65" priority="17">
+    <cfRule type="expression" dxfId="63" priority="17">
       <formula>$G4="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="18">
+    <cfRule type="expression" dxfId="62" priority="18">
       <formula>$G4="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F3">
-    <cfRule type="expression" dxfId="63" priority="15">
+    <cfRule type="expression" dxfId="61" priority="15">
       <formula>$G3="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="16">
+    <cfRule type="expression" dxfId="60" priority="16">
       <formula>$G3="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="61" priority="13">
+    <cfRule type="expression" dxfId="59" priority="13">
       <formula>$G2="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>$G2="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="59" priority="11">
+    <cfRule type="expression" dxfId="57" priority="11">
       <formula>$G6="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="12">
+    <cfRule type="expression" dxfId="56" priority="12">
       <formula>$G6="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="57" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>$G7="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="10">
+    <cfRule type="expression" dxfId="54" priority="10">
       <formula>$G7="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="55" priority="7">
+    <cfRule type="expression" dxfId="53" priority="7">
       <formula>$G8="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="8">
+    <cfRule type="expression" dxfId="52" priority="8">
       <formula>$G8="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>"closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="49" priority="3">
       <formula>$G29="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="48" priority="4">
       <formula>$G29="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>$G29="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>$G29="closed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2600,10 +2149,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>8</v>
@@ -2611,13 +2160,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2747,13 +2296,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2768,186 +2317,186 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{21B7E40D-2FBA-4FF4-B35F-30341514E5CB}"/>
   <conditionalFormatting sqref="G2 G4:G28">
-    <cfRule type="cellIs" dxfId="53" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:F28">
-    <cfRule type="expression" dxfId="51" priority="45">
+    <cfRule type="expression" dxfId="43" priority="45">
       <formula>$G15="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="46">
+    <cfRule type="expression" dxfId="42" priority="46">
       <formula>$G15="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:F14">
-    <cfRule type="expression" dxfId="49" priority="43">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>$G14="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="44">
+    <cfRule type="expression" dxfId="40" priority="44">
       <formula>$G14="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:F13">
-    <cfRule type="expression" dxfId="47" priority="41">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>$G13="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42">
+    <cfRule type="expression" dxfId="38" priority="42">
       <formula>$G13="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:F12">
-    <cfRule type="expression" dxfId="45" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>$G12="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="40">
+    <cfRule type="expression" dxfId="36" priority="40">
       <formula>$G12="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:F11">
-    <cfRule type="expression" dxfId="43" priority="37">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>$G11="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
+    <cfRule type="expression" dxfId="34" priority="38">
       <formula>$G11="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:F10">
-    <cfRule type="expression" dxfId="41" priority="35">
+    <cfRule type="expression" dxfId="33" priority="35">
       <formula>$G10="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="36">
+    <cfRule type="expression" dxfId="32" priority="36">
       <formula>$G10="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:F9">
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>$G9="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="30" priority="34">
       <formula>$G9="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 E8:F8">
-    <cfRule type="expression" dxfId="37" priority="31">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>$G8="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="32">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>$G8="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C7 E7:F7">
-    <cfRule type="expression" dxfId="35" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>$G7="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>$G7="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:C6 E6:F6">
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$G6="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>$G6="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:F5">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>$G5="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>$G5="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="29" priority="23">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>$G4="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="24">
+    <cfRule type="expression" dxfId="20" priority="24">
       <formula>$G4="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="19" priority="19">
       <formula>$G2="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>$G2="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="17" priority="17">
       <formula>$G6="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>$G6="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>$G7="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>$G7="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>$G8="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>$G8="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:F3">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>$G3="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>$G3="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$G3="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$G3="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$G29="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$G29="closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$G29="open"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$G29="closed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>